<commit_message>
performed t-tests on accelerometer versus gyroscope results
</commit_message>
<xml_diff>
--- a/Evaluation/bodyweight_vs_weighted_bal_acc.xlsx
+++ b/Evaluation/bodyweight_vs_weighted_bal_acc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\ExerciseClassification\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98A1969-869A-4E62-9A9E-2586B65D046F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BC7D10-2228-4120-8810-AAC8E2408552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28515" yWindow="855" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mean Balance Accuracy" sheetId="1" r:id="rId1"/>
@@ -218,9 +218,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -308,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -325,12 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,34 +615,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -655,7 +657,7 @@
         <v>0.17958333333333398</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>50</v>
       </c>
@@ -670,7 +672,7 @@
         <v>1.1250000000000981E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -685,7 +687,7 @@
         <v>0.31624999999999903</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
@@ -700,7 +702,7 @@
         <v>0.13833333333333309</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
@@ -715,7 +717,7 @@
         <v>2.3750000000000049E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
@@ -730,7 +732,7 @@
         <v>6.3749999999998974E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
@@ -745,7 +747,7 @@
         <v>4.2916666666666048E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
@@ -760,7 +762,7 @@
         <v>8.7500000000000022E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -775,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -803,9 +805,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -823,7 +825,7 @@
         <v>8.7499999999999897E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -846,7 +848,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.93333333333333302</v>
       </c>
@@ -866,7 +868,7 @@
         <v>3.6180615518727408</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -892,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -914,7 +916,7 @@
         <v>0.88250000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -936,7 +938,7 @@
         <v>2.7499999999999981E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.85</v>
       </c>
@@ -958,7 +960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -978,7 +980,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -998,7 +1000,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1018,7 +1020,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1038,7 +1040,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1047,7 +1049,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -1056,7 +1058,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -1065,7 +1067,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -1074,37 +1076,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1124,9 +1126,9 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1167,7 +1169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1187,7 +1189,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1257,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1279,7 +1281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -1299,7 +1301,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1319,7 +1321,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1339,7 +1341,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1359,7 +1361,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1368,7 +1370,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -1377,7 +1379,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -1386,7 +1388,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -1395,37 +1397,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1445,9 +1447,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>5.7083333333333305E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.93333333333333302</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>2.1442051540444638</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1556,7 +1558,7 @@
         <v>0.93625000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>6.4392361111111109E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1600,7 +1602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -1620,7 +1622,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1640,7 +1642,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1660,7 +1662,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1680,7 +1682,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1689,7 +1691,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -1698,7 +1700,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -1707,7 +1709,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -1716,37 +1718,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1762,20 +1764,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24600D9A-CF85-447A-B680-EBC46EFD1876}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>47</v>
@@ -1790,170 +1792,170 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="14">
         <v>0.17958333333333321</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="14">
         <v>0.27536066416678046</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="14">
         <v>2.062358343218587</v>
       </c>
       <c r="E2" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="14">
         <v>1.1250000000000005E-2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="14">
         <v>2.3899383999499986E-2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="14">
         <v>1.4885581853339227</v>
       </c>
       <c r="E3" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="14">
         <v>0.31888888888888889</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="14">
         <v>0.14687415177935625</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="14">
         <v>6.8658453321599824</v>
       </c>
       <c r="E4" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="14">
         <v>0.138333333333333</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="14">
         <v>9.1851665173048172E-2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="14">
         <v>4.7625528490144884</v>
       </c>
       <c r="E5" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="14">
         <v>2.3750000000000004E-2</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="14">
         <v>4.2675292096897896E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="14">
         <v>1.7598964351191495</v>
       </c>
       <c r="E6" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="14">
         <v>6.374999999999971E-2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="14">
         <v>0.10932681919392764</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="14">
         <v>1.8439684088689785</v>
       </c>
       <c r="E7" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="14">
         <v>4.2916666666666291E-2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="14">
         <v>0.11137208933997166</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="14">
         <v>1.2185675697850411</v>
       </c>
       <c r="E8" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="14">
         <v>8.7499999999999897E-2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="14">
         <v>7.6477221655201211E-2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="14">
         <v>3.6180615518727408</v>
       </c>
       <c r="E9" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
         <v>0</v>
       </c>
       <c r="E10" s="7">
         <v>2.262</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="14">
         <v>5.7083333333333305E-2</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="14">
         <v>8.4186603799293755E-2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="14">
         <v>2.1442051540444638</v>
       </c>
       <c r="E11" s="7">
@@ -1973,15 +1975,15 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1999,7 +2001,7 @@
         <v>0.17958333333333321</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0.46666666666666601</v>
       </c>
@@ -2022,7 +2024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.266666666666666</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>2.062358343218587</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.85</v>
       </c>
@@ -2090,7 +2092,7 @@
         <v>0.49874999999999992</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>1.0467013888888932E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.5</v>
       </c>
@@ -2134,7 +2136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>0.85</v>
       </c>
@@ -2154,7 +2156,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>0.7</v>
       </c>
@@ -2174,7 +2176,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.3</v>
       </c>
@@ -2194,7 +2196,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -2214,7 +2216,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2223,7 +2225,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -2232,7 +2234,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -2241,7 +2243,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -2250,37 +2252,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2301,9 +2303,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2323,7 @@
         <v>1.1250000000000005E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2344,7 +2346,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>1.4885581853339227</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -2390,7 +2392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2412,7 +2414,7 @@
         <v>0.98874999999999991</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v>5.7118055555555589E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -2456,7 +2458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -2476,7 +2478,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -2496,7 +2498,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2516,7 +2518,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -2536,7 +2538,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2545,7 +2547,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -2554,7 +2556,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -2563,7 +2565,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -2572,37 +2574,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2622,9 +2624,9 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2642,7 +2644,7 @@
         <v>0.31888888888888889</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.86666666666666603</v>
       </c>
@@ -2685,7 +2687,7 @@
         <v>6.8658453321599824</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>0.85</v>
       </c>
@@ -2711,7 +2713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.85</v>
       </c>
@@ -2733,7 +2735,7 @@
         <v>0.56111111111111067</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -2755,7 +2757,7 @@
         <v>6.4814814814814587E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.68333333333333302</v>
       </c>
@@ -2777,7 +2779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>0.78333333333333299</v>
       </c>
@@ -2797,7 +2799,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -2817,7 +2819,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -2837,7 +2839,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -2857,7 +2859,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2866,7 +2868,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -2875,7 +2877,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -2884,7 +2886,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -2893,37 +2895,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2943,9 +2945,9 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2963,7 +2965,7 @@
         <v>0.1383333333333332</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>4.7625528490144884</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -3032,7 +3034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -3054,7 +3056,7 @@
         <v>0.83000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>6.7083333333333309E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.83333333333333304</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -3118,7 +3120,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -3138,7 +3140,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -3158,7 +3160,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -3178,7 +3180,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -3187,7 +3189,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -3196,7 +3198,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -3205,7 +3207,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -3214,37 +3216,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3264,9 +3266,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3284,7 +3286,7 @@
         <v>2.3750000000000004E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3307,7 +3309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -3327,7 +3329,7 @@
         <v>1.7598964351191495</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>0.97624999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>1.8211805555555559E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -3419,7 +3421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -3439,7 +3441,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -3459,7 +3461,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -3479,7 +3481,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -3499,7 +3501,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -3508,7 +3510,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -3517,7 +3519,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -3526,7 +3528,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -3535,37 +3537,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3585,9 +3587,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>6.374999999999971E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -3628,7 +3630,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.86666666666666603</v>
       </c>
@@ -3648,7 +3650,7 @@
         <v>1.8439684088689785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -3674,7 +3676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -3696,7 +3698,7 @@
         <v>0.83125000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>0.86666666666666603</v>
       </c>
@@ -3718,7 +3720,7 @@
         <v>6.1545138888889116E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.68333333333333302</v>
       </c>
@@ -3740,7 +3742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>0.83333333333333304</v>
       </c>
@@ -3760,7 +3762,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -3780,7 +3782,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -3800,7 +3802,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -3820,7 +3822,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -3829,7 +3831,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -3838,7 +3840,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -3847,7 +3849,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -3856,37 +3858,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3906,9 +3908,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3926,7 +3928,7 @@
         <v>4.2916666666666291E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -3949,7 +3951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>0.78333333333333299</v>
       </c>
@@ -3969,7 +3971,7 @@
         <v>1.2185675697850411</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -3995,7 +3997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.91666666666666596</v>
       </c>
@@ -4017,7 +4019,7 @@
         <v>0.81874999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>4.9392361111111104E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>0.68333333333333302</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -4081,7 +4083,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>0.86666666666666603</v>
       </c>
@@ -4101,7 +4103,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.63333333333333297</v>
       </c>
@@ -4121,7 +4123,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>0.93333333333333302</v>
       </c>
@@ -4141,7 +4143,7 @@
       </c>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="8" t="s">
         <v>43</v>
       </c>
@@ -4150,7 +4152,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="8" t="s">
         <v>44</v>
       </c>
@@ -4159,7 +4161,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="8" t="s">
         <v>45</v>
       </c>
@@ -4168,7 +4170,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" s="9" t="s">
         <v>46</v>
       </c>
@@ -4177,37 +4179,37 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>